<commit_message>
update legacy GBSL importer
</commit_message>
<xml_diff>
--- a/tests/integration/stubs/terminplan-gbsl.xlsx
+++ b/tests/integration/stubs/terminplan-gbsl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\balz\git_code\lebalz\events-api\tests\integration\stubs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9ECAA7-3FA9-4B11-8571-6F6F1D067DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00415293-A99D-4118-883B-09DA6795467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="950" yWindow="1000" windowWidth="28800" windowHeight="15410" xr2:uid="{E273EB81-F009-42CB-8811-F9066D4F90FA}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{E273EB81-F009-42CB-8811-F9066D4F90FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>KW</t>
   </si>
@@ -132,19 +132,29 @@
   </si>
   <si>
     <t>KLP</t>
+  </si>
+  <si>
+    <t>betrifft  (0=KL; 1=LP; 2=SuS; 3=alle)</t>
+  </si>
+  <si>
+    <t>Unterricht betroffen (0=nein; 1= teilweise; 2=ja)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Textkörper)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -163,14 +173,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -487,19 +515,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7971152F-4D71-40FF-839F-4423C8E59447}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="59.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="93">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,8 +574,14 @@
       <c r="O1" t="s">
         <v>12</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>34</v>
       </c>
@@ -571,8 +606,14 @@
       <c r="L2" t="s">
         <v>18</v>
       </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17">
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -597,8 +638,14 @@
       <c r="K3" t="s">
         <v>17</v>
       </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -632,8 +679,14 @@
       <c r="O4" t="s">
         <v>28</v>
       </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>35</v>
       </c>
@@ -666,8 +719,12 @@
       <c r="O5" t="s">
         <v>27</v>
       </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>